<commit_message>
The contriction parser reference column on the excel can be configured.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sinFechas_2.xlsx
+++ b/files/pruebas/v6_sinFechas_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267B1B6C-D779-4CA1-8DA8-5EBA3893B768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E311C02-40F5-4889-8A76-8D1BE6824AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13230" yWindow="4680" windowWidth="26430" windowHeight="15180" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13230" yWindow="4680" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -1279,9 +1279,6 @@
     <t>Distancia temporal entre exámenes</t>
   </si>
   <si>
-    <t>Exaámenes en el mismo día.</t>
-  </si>
-  <si>
     <t>Día prohibido para examen</t>
   </si>
   <si>
@@ -1301,6 +1298,9 @@
   </si>
   <si>
     <t>DD</t>
+  </si>
+  <si>
+    <t>Exámenes en el mismo día.</t>
   </si>
 </sst>
 </file>
@@ -1902,9 +1902,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6532,220 +6530,207 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="B2:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B21"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="97" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="97" t="s">
         <v>388</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>383</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>384</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="C6">
         <v>45</v>
       </c>
-      <c r="C5">
+      <c r="D6">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>47</v>
       </c>
-      <c r="B6">
+      <c r="C7">
         <v>34</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1</v>
+      </c>
       <c r="E7" s="93"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="97" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="97" t="s">
         <v>381</v>
       </c>
-      <c r="B9" s="97"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="97" t="s">
-        <v>389</v>
-      </c>
-      <c r="B10" s="97"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C10" s="97"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="97" t="s">
+        <v>396</v>
+      </c>
+      <c r="C11" s="97"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>383</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C12" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>46</v>
-      </c>
-      <c r="B12">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>34</v>
-      </c>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="C13">
         <v>47</v>
       </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>47</v>
+      </c>
+      <c r="C15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="97" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="97" t="s">
         <v>382</v>
       </c>
-      <c r="B16" s="97"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
+      <c r="C17" s="97"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="97" t="s">
+        <v>389</v>
+      </c>
+      <c r="C18" s="97"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="95" t="s">
+        <v>386</v>
+      </c>
+      <c r="C19" s="95" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>23</v>
+      </c>
+      <c r="C20" s="30">
+        <v>44364</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="97" t="s">
+        <v>395</v>
+      </c>
+      <c r="C22" s="97"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="97" t="s">
         <v>390</v>
       </c>
-      <c r="B17" s="97"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="95" t="s">
-        <v>386</v>
-      </c>
-      <c r="B18" s="95" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="C23" s="97"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>383</v>
+      </c>
+      <c r="C24" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25">
         <v>23</v>
       </c>
-      <c r="B19" s="30">
-        <v>44364</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="97" t="s">
-        <v>396</v>
-      </c>
-      <c r="B21" s="97"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="97" t="s">
+      <c r="C25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="97" t="s">
         <v>391</v>
       </c>
-      <c r="B22" s="97"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>383</v>
-      </c>
-      <c r="B23" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="C27" s="97"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="97" t="s">
+        <v>392</v>
+      </c>
+      <c r="C28" s="97"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>393</v>
+      </c>
+      <c r="C29" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="97" t="s">
-        <v>392</v>
-      </c>
-      <c r="B26" s="97"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="97" t="s">
-        <v>393</v>
-      </c>
-      <c r="B27" s="97"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>394</v>
-      </c>
-      <c r="B28" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>23</v>
-      </c>
-      <c r="B29">
+      <c r="C30">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A16:B16"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Output schedules now provide the constrictions specifying which are fulfilled in the scheduling.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sinFechas_2.xlsx
+++ b/files/pruebas/v6_sinFechas_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA70F47-785E-40BA-8FFE-7752BE12C85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4097E6EE-1C11-4256-A557-3A03CBC66903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="420" windowWidth="26430" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="399">
   <si>
     <t>ID</t>
   </si>
@@ -1304,6 +1304,9 @@
   </si>
   <si>
     <t>Tiempo Extra</t>
+  </si>
+  <si>
+    <t>Cumplida?</t>
   </si>
 </sst>
 </file>
@@ -1426,7 +1429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1811,11 +1814,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1909,17 +1977,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1933,27 +1993,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2419,7 +2491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
@@ -2523,10 +2595,10 @@
       <c r="Q5" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="101" t="s">
+      <c r="R5" s="97" t="s">
         <v>299</v>
       </c>
-      <c r="S5" s="101"/>
+      <c r="S5" s="97"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
@@ -5549,7 +5621,7 @@
       <c r="J50" s="15">
         <v>0.10416666666666667</v>
       </c>
-      <c r="K50" s="94"/>
+      <c r="K50" s="93"/>
       <c r="L50" s="7" t="str">
         <f t="shared" si="2"/>
         <v>sábado</v>
@@ -6775,10 +6847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
-  <dimension ref="B2:E37"/>
+  <dimension ref="B2:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6789,232 +6861,286 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="105" t="s">
         <v>380</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="104"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="105" t="s">
         <v>388</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="107"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="106" t="s">
         <v>383</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="106" t="s">
         <v>384</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="106" t="s">
         <v>385</v>
       </c>
+      <c r="E4" s="107" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="39">
+      <c r="B5" s="101">
         <v>0</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="40">
-        <v>1</v>
-      </c>
+      <c r="D5" s="101">
+        <v>1</v>
+      </c>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="39">
+      <c r="B6" s="102">
         <v>5</v>
       </c>
       <c r="C6" s="5">
         <v>45</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="102">
         <v>2</v>
       </c>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="39">
+      <c r="B7" s="102">
         <v>47</v>
       </c>
       <c r="C7" s="5">
         <v>34</v>
       </c>
-      <c r="D7" s="40">
-        <v>1</v>
-      </c>
-      <c r="E7" s="93"/>
+      <c r="D7" s="102">
+        <v>1</v>
+      </c>
+      <c r="E7" s="104"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="95"/>
+      <c r="B8" s="108"/>
       <c r="C8" s="71"/>
-      <c r="D8" s="85"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="85"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="102" t="s">
+      <c r="B10" s="98" t="s">
         <v>381</v>
       </c>
-      <c r="C10" s="104"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="100"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="115" t="s">
         <v>396</v>
       </c>
-      <c r="C11" s="107"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="117"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="118" t="s">
         <v>383</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="119" t="s">
         <v>384</v>
+      </c>
+      <c r="D12" s="114" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="39">
         <v>46</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="101">
         <v>47</v>
       </c>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="39">
         <v>34</v>
       </c>
-      <c r="C14" s="40">
+      <c r="C14" s="102">
         <v>46</v>
       </c>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="39">
         <v>47</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="102">
         <v>3</v>
       </c>
+      <c r="D15" s="104"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="95"/>
-      <c r="C16" s="85"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="102" t="s">
+      <c r="B16" s="94"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="85"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="105" t="s">
         <v>382</v>
       </c>
-      <c r="C19" s="104"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="105"/>
+      <c r="D19" s="105"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="105" t="s">
         <v>389</v>
       </c>
-      <c r="C20" s="107"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="96" t="s">
+      <c r="C20" s="105"/>
+      <c r="D20" s="105"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="111" t="s">
         <v>386</v>
       </c>
-      <c r="C21" s="97" t="s">
+      <c r="C21" s="111" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="39">
+      <c r="D21" s="107" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="101">
         <v>23</v>
       </c>
-      <c r="C22" s="98">
+      <c r="C22" s="95">
         <v>44364</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="99"/>
-      <c r="C23" s="100"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="101"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="112"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="113"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" s="30"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="102" t="s">
+      <c r="D24" s="5"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="105" t="s">
         <v>395</v>
       </c>
-      <c r="C26" s="104"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="105"/>
+      <c r="D26" s="105"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="105" t="s">
         <v>390</v>
       </c>
-      <c r="C27" s="107"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="39" t="s">
+      <c r="C27" s="105"/>
+      <c r="D27" s="105"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="106" t="s">
         <v>383</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="106" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="39">
+      <c r="D28" s="107" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="101">
         <v>23</v>
       </c>
       <c r="C29" s="40">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="95"/>
+      <c r="D29" s="40"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="108"/>
       <c r="C30" s="85"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="85"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="110" t="s">
+      <c r="D31" s="103"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="109" t="s">
         <v>391</v>
       </c>
-      <c r="C33" s="111"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="108" t="s">
+      <c r="C33" s="109"/>
+      <c r="D33" s="109"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="110" t="s">
         <v>392</v>
       </c>
-      <c r="C34" s="109"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="39" t="s">
+      <c r="C34" s="110"/>
+      <c r="D34" s="110"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="106" t="s">
         <v>393</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="106" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="39">
+      <c r="D35" s="107" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="101">
         <v>23</v>
       </c>
       <c r="C36" s="40">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="95"/>
+      <c r="D36" s="102"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="108"/>
       <c r="C37" s="85"/>
+      <c r="D37" s="108"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="103"/>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
User Constrictions can now be Hard instead of Weak on user demand.
New Configuration file added: hardConstrictions
New hierarchy for Constrictions, HardifiableConstriction.java
Fixed a bug in TimeDisplacementConstriction.java
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sinFechas_2.xlsx
+++ b/files/pruebas/v6_sinFechas_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4097E6EE-1C11-4256-A557-3A03CBC66903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24DCA6E-EF66-4CE9-8DEF-414BCAFA7704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="420" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -1981,8 +1981,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1993,95 +2020,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2144,6 +2093,57 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2170,23 +2170,23 @@
     <sortCondition ref="F2:F34"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="11"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="19"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2595,10 +2595,10 @@
       <c r="Q5" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="97" t="s">
+      <c r="R5" s="110" t="s">
         <v>299</v>
       </c>
-      <c r="S5" s="97"/>
+      <c r="S5" s="110"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
@@ -6810,32 +6810,32 @@
     <mergeCell ref="R5:S5"/>
   </mergeCells>
   <conditionalFormatting sqref="R10 R8:S9 R11:S33 R34 R35:S67 A7:N43 A6:J6 L6:S6 A45:N57 A44:J44 L44:N44 A59:N67 A58:J58 L58:N58 P8:Q67 P7:S7 O7:O67">
-    <cfRule type="expression" dxfId="24" priority="18">
+    <cfRule type="expression" dxfId="7" priority="18">
       <formula>$T6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H67">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Presencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6:R67">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"polideportivo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$R6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$R44=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$R58=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6847,10 +6847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
-  <dimension ref="B2:E40"/>
+  <dimension ref="B2:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6861,286 +6861,829 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="111" t="s">
         <v>380</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="111" t="s">
         <v>388</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="101" t="s">
         <v>383</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="C4" s="101" t="s">
         <v>384</v>
       </c>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="E4" s="107" t="s">
+      <c r="E4" s="102" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="101">
+      <c r="B5" s="97">
         <v>0</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="101">
+      <c r="D5" s="97">
         <v>1</v>
       </c>
       <c r="E5" s="40"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="102">
+      <c r="B6" s="98">
         <v>5</v>
       </c>
       <c r="C6" s="5">
         <v>45</v>
       </c>
-      <c r="D6" s="102">
+      <c r="D6" s="98">
         <v>2</v>
       </c>
       <c r="E6" s="40"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="102">
+      <c r="B7" s="98">
         <v>47</v>
       </c>
       <c r="C7" s="5">
         <v>34</v>
       </c>
-      <c r="D7" s="102">
-        <v>1</v>
-      </c>
-      <c r="E7" s="104"/>
+      <c r="D7" s="98">
+        <v>1</v>
+      </c>
+      <c r="E7" s="100"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="108"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="85"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="98" t="s">
-        <v>381</v>
-      </c>
-      <c r="C10" s="99"/>
-      <c r="D10" s="100"/>
+      <c r="B8" s="98">
+        <v>0</v>
+      </c>
+      <c r="C8" s="36">
+        <v>50</v>
+      </c>
+      <c r="D8" s="98">
+        <v>18</v>
+      </c>
+      <c r="E8" s="100"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="103"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="85"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="115" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="C11" s="116"/>
       <c r="D11" s="117"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="112" t="s">
+        <v>396</v>
+      </c>
+      <c r="C12" s="113"/>
+      <c r="D12" s="114"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="108" t="s">
         <v>383</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C13" s="109" t="s">
         <v>384</v>
       </c>
-      <c r="D12" s="114" t="s">
+      <c r="D13" s="107" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="39">
-        <v>46</v>
-      </c>
-      <c r="C13" s="101">
-        <v>47</v>
-      </c>
-      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="39">
-        <v>34</v>
-      </c>
-      <c r="C14" s="102">
         <v>46</v>
+      </c>
+      <c r="C14" s="97">
+        <v>47</v>
       </c>
       <c r="D14" s="40"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="39">
+        <v>34</v>
+      </c>
+      <c r="C15" s="98">
+        <v>46</v>
+      </c>
+      <c r="D15" s="40"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="39">
         <v>47</v>
       </c>
-      <c r="C15" s="102">
+      <c r="C16" s="98">
         <v>3</v>
       </c>
-      <c r="D15" s="104"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="94"/>
-      <c r="C16" s="108"/>
-      <c r="D16" s="85"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="105" t="s">
+      <c r="D16" s="100"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="94"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="85"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="111" t="s">
         <v>382</v>
       </c>
-      <c r="C19" s="105"/>
-      <c r="D19" s="105"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="105" t="s">
-        <v>389</v>
-      </c>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
+      <c r="C20" s="111"/>
+      <c r="D20" s="111"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="111" t="s">
+        <v>389</v>
+      </c>
+      <c r="C21" s="111"/>
+      <c r="D21" s="111"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="104" t="s">
         <v>386</v>
       </c>
-      <c r="C21" s="111" t="s">
+      <c r="C22" s="104" t="s">
         <v>387</v>
       </c>
-      <c r="D21" s="107" t="s">
+      <c r="D22" s="102" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="101">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="97">
+        <v>1</v>
+      </c>
+      <c r="C23" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D23" s="97"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="98">
+        <v>2</v>
+      </c>
+      <c r="C24" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D24" s="98"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="97">
+        <v>3</v>
+      </c>
+      <c r="C25" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D25" s="98"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="98">
+        <v>4</v>
+      </c>
+      <c r="C26" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D26" s="98"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="97">
+        <v>5</v>
+      </c>
+      <c r="C27" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D27" s="98"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="98">
+        <v>6</v>
+      </c>
+      <c r="C28" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D28" s="98"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="97">
+        <v>7</v>
+      </c>
+      <c r="C29" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D29" s="98"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="98">
+        <v>8</v>
+      </c>
+      <c r="C30" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D30" s="98"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="97">
+        <v>9</v>
+      </c>
+      <c r="C31" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D31" s="98"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="98">
+        <v>10</v>
+      </c>
+      <c r="C32" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D32" s="98"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="97">
+        <v>11</v>
+      </c>
+      <c r="C33" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D33" s="98"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="98">
+        <v>12</v>
+      </c>
+      <c r="C34" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D34" s="98"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="97">
+        <v>13</v>
+      </c>
+      <c r="C35" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D35" s="98"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="98">
+        <v>14</v>
+      </c>
+      <c r="C36" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D36" s="98"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="97">
+        <v>15</v>
+      </c>
+      <c r="C37" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D37" s="98"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="98">
+        <v>16</v>
+      </c>
+      <c r="C38" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D38" s="98"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="97">
+        <v>17</v>
+      </c>
+      <c r="C39" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D39" s="98"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="98">
+        <v>18</v>
+      </c>
+      <c r="C40" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D40" s="98"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="97">
+        <v>19</v>
+      </c>
+      <c r="C41" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D41" s="98"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="98">
+        <v>20</v>
+      </c>
+      <c r="C42" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D42" s="98"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="97">
+        <v>21</v>
+      </c>
+      <c r="C43" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D43" s="98"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="98">
+        <v>22</v>
+      </c>
+      <c r="C44" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D44" s="98"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="97">
         <v>23</v>
       </c>
-      <c r="C22" s="95">
+      <c r="C45" s="95">
         <v>44364</v>
       </c>
-      <c r="D22" s="101"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="112"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="113"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="30"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="105" t="s">
+      <c r="D45" s="98"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="98">
+        <v>24</v>
+      </c>
+      <c r="C46" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D46" s="98"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="97">
+        <v>25</v>
+      </c>
+      <c r="C47" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D47" s="98"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="98">
+        <v>26</v>
+      </c>
+      <c r="C48" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D48" s="98"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="97">
+        <v>27</v>
+      </c>
+      <c r="C49" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D49" s="98"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="98">
+        <v>28</v>
+      </c>
+      <c r="C50" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D50" s="98"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="97">
+        <v>29</v>
+      </c>
+      <c r="C51" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D51" s="98"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="98">
+        <v>30</v>
+      </c>
+      <c r="C52" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D52" s="98"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="97">
+        <v>31</v>
+      </c>
+      <c r="C53" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D53" s="98"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="98">
+        <v>32</v>
+      </c>
+      <c r="C54" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D54" s="98"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="97">
+        <v>33</v>
+      </c>
+      <c r="C55" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D55" s="98"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="98">
+        <v>34</v>
+      </c>
+      <c r="C56" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D56" s="98"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="97">
+        <v>35</v>
+      </c>
+      <c r="C57" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D57" s="98"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="98">
+        <v>36</v>
+      </c>
+      <c r="C58" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D58" s="98"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="97">
+        <v>37</v>
+      </c>
+      <c r="C59" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D59" s="98"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="98">
+        <v>38</v>
+      </c>
+      <c r="C60" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D60" s="98"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="97">
+        <v>39</v>
+      </c>
+      <c r="C61" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D61" s="98"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="98">
+        <v>40</v>
+      </c>
+      <c r="C62" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D62" s="98"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="97">
+        <v>41</v>
+      </c>
+      <c r="C63" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D63" s="98"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="98">
+        <v>42</v>
+      </c>
+      <c r="C64" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D64" s="98"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="97">
+        <v>43</v>
+      </c>
+      <c r="C65" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D65" s="98"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="98">
+        <v>44</v>
+      </c>
+      <c r="C66" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D66" s="98"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="97">
+        <v>45</v>
+      </c>
+      <c r="C67" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D67" s="98"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="98">
+        <v>46</v>
+      </c>
+      <c r="C68" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D68" s="98"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="97">
+        <v>47</v>
+      </c>
+      <c r="C69" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D69" s="98"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="98">
+        <v>48</v>
+      </c>
+      <c r="C70" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D70" s="98"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="97">
+        <v>49</v>
+      </c>
+      <c r="C71" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D71" s="98"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="98">
+        <v>50</v>
+      </c>
+      <c r="C72" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D72" s="98"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="97">
+        <v>51</v>
+      </c>
+      <c r="C73" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D73" s="98"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="98">
+        <v>52</v>
+      </c>
+      <c r="C74" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D74" s="98"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="97">
+        <v>53</v>
+      </c>
+      <c r="C75" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D75" s="98"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="98">
+        <v>54</v>
+      </c>
+      <c r="C76" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D76" s="98"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="97">
+        <v>55</v>
+      </c>
+      <c r="C77" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D77" s="98"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="98">
+        <v>56</v>
+      </c>
+      <c r="C78" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D78" s="98"/>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="97">
+        <v>57</v>
+      </c>
+      <c r="C79" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D79" s="98"/>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="98">
+        <v>58</v>
+      </c>
+      <c r="C80" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D80" s="98"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="97">
+        <v>59</v>
+      </c>
+      <c r="C81" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D81" s="98"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="98">
+        <v>60</v>
+      </c>
+      <c r="C82" s="95">
+        <v>44364</v>
+      </c>
+      <c r="D82" s="98"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="105"/>
+      <c r="C83" s="96"/>
+      <c r="D83" s="106"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C84" s="30"/>
+      <c r="D84" s="5"/>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="111" t="s">
         <v>395</v>
       </c>
-      <c r="C26" s="105"/>
-      <c r="D26" s="105"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="105" t="s">
+      <c r="C86" s="111"/>
+      <c r="D86" s="111"/>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="111" t="s">
         <v>390</v>
       </c>
-      <c r="C27" s="105"/>
-      <c r="D27" s="105"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="106" t="s">
+      <c r="C87" s="111"/>
+      <c r="D87" s="111"/>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="101" t="s">
         <v>383</v>
       </c>
-      <c r="C28" s="106" t="s">
+      <c r="C88" s="101" t="s">
         <v>384</v>
       </c>
-      <c r="D28" s="107" t="s">
+      <c r="D88" s="102" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="101">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="97">
         <v>23</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C89" s="40">
         <v>24</v>
       </c>
-      <c r="D29" s="40"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="108"/>
-      <c r="C30" s="85"/>
-      <c r="D30" s="85"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="103"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="109" t="s">
+      <c r="D89" s="40"/>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="103"/>
+      <c r="C90" s="85"/>
+      <c r="D90" s="85"/>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="99"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="119" t="s">
         <v>391</v>
       </c>
-      <c r="C33" s="109"/>
-      <c r="D33" s="109"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="110" t="s">
+      <c r="C93" s="119"/>
+      <c r="D93" s="119"/>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="118" t="s">
         <v>392</v>
       </c>
-      <c r="C34" s="110"/>
-      <c r="D34" s="110"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="106" t="s">
+      <c r="C94" s="118"/>
+      <c r="D94" s="118"/>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="101" t="s">
         <v>393</v>
       </c>
-      <c r="C35" s="106" t="s">
+      <c r="C95" s="101" t="s">
         <v>394</v>
       </c>
-      <c r="D35" s="107" t="s">
+      <c r="D95" s="102" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="101">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="97">
         <v>23</v>
       </c>
-      <c r="C36" s="40">
+      <c r="C96" s="40">
         <v>26</v>
       </c>
-      <c r="D36" s="102"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="108"/>
-      <c r="C37" s="85"/>
-      <c r="D37" s="108"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D38" s="103"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D40" s="5"/>
+      <c r="D96" s="98"/>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="103"/>
+      <c r="C97" s="85"/>
+      <c r="D97" s="103"/>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D98" s="99"/>
+      <c r="E98" s="5"/>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D100" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B10:D10"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7152,7 +7695,7 @@
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7247,7 +7790,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7443,7 +7986,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C16">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Changed Constriction class Hierarchy.
The new approach provides support for both Hard and Weak Constrictions, and for weak contrictions that can be marked as hard by the user. This last type of constrictions are UserConstriction.java.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sinFechas_2.xlsx
+++ b/files/pruebas/v6_sinFechas_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24DCA6E-EF66-4CE9-8DEF-414BCAFA7704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB23ED0B-5CE1-4930-8ABB-E7FD39330AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2370" yWindow="420" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2002,6 +2002,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2020,17 +2026,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2093,57 +2144,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2170,23 +2170,23 @@
     <sortCondition ref="F2:F34"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="19"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6810,32 +6810,32 @@
     <mergeCell ref="R5:S5"/>
   </mergeCells>
   <conditionalFormatting sqref="R10 R8:S9 R11:S33 R34 R35:S67 A7:N43 A6:J6 L6:S6 A45:N57 A44:J44 L44:N44 A59:N67 A58:J58 L58:N58 P8:Q67 P7:S7 O7:O67">
-    <cfRule type="expression" dxfId="7" priority="18">
+    <cfRule type="expression" dxfId="24" priority="18">
       <formula>$T6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H67">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>"Presencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6:R67">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"polideportivo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>$R6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>$R44=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>$R58=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6850,7 +6850,7 @@
   <dimension ref="B2:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6919,7 +6919,7 @@
         <v>47</v>
       </c>
       <c r="C7" s="5">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D7" s="98">
         <v>1</v>
@@ -6934,7 +6934,7 @@
         <v>50</v>
       </c>
       <c r="D8" s="98">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E8" s="100"/>
     </row>
@@ -6945,18 +6945,18 @@
       <c r="E9" s="85"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="115" t="s">
+      <c r="B11" s="117" t="s">
         <v>381</v>
       </c>
-      <c r="C11" s="116"/>
-      <c r="D11" s="117"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="119"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="114" t="s">
         <v>396</v>
       </c>
-      <c r="C12" s="113"/>
-      <c r="D12" s="114"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="116"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="108" t="s">
@@ -7623,18 +7623,18 @@
       <c r="D92" s="5"/>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="119" t="s">
+      <c r="B93" s="113" t="s">
         <v>391</v>
       </c>
-      <c r="C93" s="119"/>
-      <c r="D93" s="119"/>
+      <c r="C93" s="113"/>
+      <c r="D93" s="113"/>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="118" t="s">
+      <c r="B94" s="112" t="s">
         <v>392</v>
       </c>
-      <c r="C94" s="118"/>
-      <c r="D94" s="118"/>
+      <c r="C94" s="112"/>
+      <c r="D94" s="112"/>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="101" t="s">
@@ -7790,7 +7790,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7986,7 +7986,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C16">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>